<commit_message>
added convert to scientific notation function
</commit_message>
<xml_diff>
--- a/10x10Output.xlsx
+++ b/10x10Output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8df1f39dcfd2574d/Desktop/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4B870EC-2786-4879-8BA3-A8042A996ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{F4B870EC-2786-4879-8BA3-A8042A996ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1F02715-DDB2-4C38-AD61-EA5A4E60C1D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1876,11 +1876,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">

</xml_diff>